<commit_message>
se sube el anvanza de las actividades
</commit_message>
<xml_diff>
--- a/Analisis/Revsion 1/Actividades.xlsx
+++ b/Analisis/Revsion 1/Actividades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Proyectos C#\rfid\Analisis\Revsion 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B32AEBF-C6F1-425F-99FB-34353155B7B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A082025-94B1-4FBA-80BE-2BB1A12E47E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4455" yWindow="4245" windowWidth="21600" windowHeight="11505" xr2:uid="{BD391B5E-42C6-4296-BC77-94B045EB933E}"/>
   </bookViews>
@@ -84,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -94,6 +94,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -110,13 +116,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -435,10 +444,13 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A9" sqref="A9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="40.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -452,24 +464,24 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -492,14 +504,14 @@
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -512,14 +524,14 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -553,17 +565,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
+    <mergeCell ref="A5:F5"/>
     <mergeCell ref="A10:G10"/>
     <mergeCell ref="A11:G11"/>
     <mergeCell ref="A7:F7"/>
     <mergeCell ref="A8:F8"/>
     <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A6:F6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>

<commit_message>
Se terminan modificaciones observadas de la revision 1
</commit_message>
<xml_diff>
--- a/Analisis/Revsion 1/Actividades.xlsx
+++ b/Analisis/Revsion 1/Actividades.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Proyectos C#\rfid\Analisis\Revsion 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aoaj720209\Documents\proyectos\RFID\Analisis\Revsion 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A082025-94B1-4FBA-80BE-2BB1A12E47E3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="4245" windowWidth="21600" windowHeight="11505" xr2:uid="{BD391B5E-42C6-4296-BC77-94B045EB933E}"/>
+    <workbookView xWindow="4455" yWindow="4245" windowWidth="21600" windowHeight="11505"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -66,7 +65,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -84,7 +83,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,6 +102,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -116,15 +121,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -440,11 +448,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF2E30D2-9066-4DAC-92A6-89EC3C447B7A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:F9"/>
+      <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,118 +472,118 @@
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A8:F8"/>
+    <mergeCell ref="A9:F9"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A5:F5"/>
-    <mergeCell ref="A10:G10"/>
-    <mergeCell ref="A11:G11"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="A8:F8"/>
-    <mergeCell ref="A9:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>